<commit_message>
new_formulation I_fa correction and definition of t_hh_cooling as power_tril()
Corretto errore in new formulation: identity_rcot deve essere devinita come flows x activities2 (e non viceversa)

In main creazione della funzione power_tril per la triangolare di raffreddamento, ma ancora non inserita tra le equazioni
</commit_message>
<xml_diff>
--- a/thesis/main/input_data/input_data.xlsx
+++ b/thesis/main/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cami/Documents/GitHub/pyesm_tesi/thesis/main/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D8C0EF-2730-A94C-B954-ABE6222A2A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBE5BBC-3DF6-C14F-8CB9-F52E2E6B5805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11620" yWindow="-28800" windowWidth="51200" windowHeight="28800" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="u" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,8 @@
     <sheet name="BEV_level_max" sheetId="19" r:id="rId19"/>
     <sheet name="BEV_level_start" sheetId="20" r:id="rId20"/>
     <sheet name="BEV_vector" sheetId="21" r:id="rId21"/>
+    <sheet name="n_hours" sheetId="22" r:id="rId22"/>
+    <sheet name="cool_factors" sheetId="23" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8808" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8852" uniqueCount="92">
   <si>
     <t>id</t>
   </si>
@@ -751,7 +753,7 @@
   <dimension ref="A1:E243"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E243"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -36624,11 +36626,281 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26B9B9E-2118-CF4D-85E6-F44771D0E818}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEAA0913-4B94-7348-94E6-5E2E72A50355}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+    <sheetView topLeftCell="A83" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>

</xml_diff>